<commit_message>
Add defects document and improve testing v2
</commit_message>
<xml_diff>
--- a/v2/documentation/Testing_v2.xlsx
+++ b/v2/documentation/Testing_v2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthew.bulley\Team-Infinite\v2\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric.diep\Desktop\Team-Infinite\Team-Infinite\v2\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9200"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="60">
   <si>
     <t>Test group 1</t>
   </si>
@@ -86,27 +86,12 @@
     <t>Requirement M3 states that the exchange IDs must be unique and in format ex:p:q</t>
   </si>
   <si>
-    <t>Output ex:0:0</t>
-  </si>
-  <si>
-    <t>Alert "Exchange ids must be different."</t>
-  </si>
-  <si>
-    <t>Alert "Exchange 2 id is invalid"</t>
-  </si>
-  <si>
-    <t>Alert "Exchange 1 id is invalid"</t>
-  </si>
-  <si>
     <t>Test Size of Grid</t>
   </si>
   <si>
     <t>Grid axis should be between 0 and 100000</t>
   </si>
   <si>
-    <t>Output ex:0:1</t>
-  </si>
-  <si>
     <t>Alert "Grid size X must be between 0 and 100000."</t>
   </si>
   <si>
@@ -119,15 +104,9 @@
     <t>Location of Exchanges must be within the grid</t>
   </si>
   <si>
-    <t>Alert "Exchange 1 location is out of range"</t>
-  </si>
-  <si>
     <t>Test Exchange Location 2</t>
   </si>
   <si>
-    <t>Alert "Exchange 2 location is out of range"</t>
-  </si>
-  <si>
     <t>Test for correct ID output</t>
   </si>
   <si>
@@ -146,36 +125,24 @@
     <t>When clicking calculate, the grid should be displayed, requirement M7</t>
   </si>
   <si>
-    <t>20 by 20 grid is displayed</t>
-  </si>
-  <si>
     <t>Test for exchange ID on displayed grid</t>
   </si>
   <si>
     <t>The Exchange ID must be shown on the displayed grid, requirement M7</t>
   </si>
   <si>
-    <t>ex:0:0 at coordinates [10,15] and ex:0:1 at coordinates [5,5]</t>
-  </si>
-  <si>
     <t>Test for distance on displayed grid</t>
   </si>
   <si>
     <t>The distance of exchange id from customer must be shown on the displayed grid, requirement M7</t>
   </si>
   <si>
-    <t>d: 25 under ex:0:0 at [10,15] and d: 10 under ex:0:1 at [5,5]</t>
-  </si>
-  <si>
     <t>Test for exchange location [0,0]</t>
   </si>
   <si>
     <t>The exchange ID and distance from customer should be shown below "home" at [0,0]</t>
   </si>
   <si>
-    <t>d: 0 shown under ex:0:0 which is shown under home at [0,0]</t>
-  </si>
-  <si>
     <t>Test for customer address on displayed grid</t>
   </si>
   <si>
@@ -188,19 +155,55 @@
     <t>100000 by 100000 grid is displayed</t>
   </si>
   <si>
-    <t>no grid displayed</t>
-  </si>
-  <si>
     <t>ex:0:0 at coordinates [0,0] and ex:0:1 at coordinates [100000,100000]</t>
   </si>
   <si>
-    <t>ex:0:0 and ex:0:1 at coordinates [5,5] with ex:0:1 below</t>
-  </si>
-  <si>
     <t>Exchange 1 ID should be above exchange 2 ID if both have the same position</t>
   </si>
   <si>
-    <t>ex:0:0 and ex:0:1 at coordinates [0,0] with ex:0:1 below ex:0:0 below home</t>
+    <t>Alert "Nearest exchange: ex:0:1, distance: 10", 20 by 20 grid is displayed</t>
+  </si>
+  <si>
+    <t>Alert "Nearest exchange: ex:0:1, distance: 5", ex:0:0 at coordinates [10,15] and ex:0:1 at coordinates [5,5]</t>
+  </si>
+  <si>
+    <t>Alert "Nearest exchange: ex:0:1, distance: 10", d: 25 under ex:0:0 at [10,15] and d: 10 under ex:0:1 at [5,5]</t>
+  </si>
+  <si>
+    <t>Alert "Nearest exchange: ex:0:0, distance: 0", d: 0 shown under ex:0:0 which is shown under home at [0,0]</t>
+  </si>
+  <si>
+    <t>Alert "Nearest exchange: ex:0:0, distance: 0", ex:0:1 at coordinates [0,0] with ex:0:1 below home</t>
+  </si>
+  <si>
+    <t>Alert "Nearest exchange: ex:0:0, distance: 10", ex:0:1 at coordinates [5,5]</t>
+  </si>
+  <si>
+    <t>Alert "Nearest exchange: ex:0:1, distance: 10"</t>
+  </si>
+  <si>
+    <t>Alert "Exchange ex:0:0 does not have a unique id."</t>
+  </si>
+  <si>
+    <t>Exchange ID does not accept a value higher than 9</t>
+  </si>
+  <si>
+    <t>Alert "Nearest exchange: ex:0:1, distance: 0"</t>
+  </si>
+  <si>
+    <t>Alert "Exchange ex:0:0 location is out of range."</t>
+  </si>
+  <si>
+    <t>Alert "Nearest exchange: ex:0:1, distance: 20"</t>
+  </si>
+  <si>
+    <t>Alert "Exchange ex:0:1 location is out of range."</t>
+  </si>
+  <si>
+    <t>Alert "Nearest exchange: ex:0:0, distance: 20"</t>
+  </si>
+  <si>
+    <t>No grid displyed, Exchange ex:0:0 location is out of range.</t>
   </si>
 </sst>
 </file>
@@ -257,7 +260,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -782,6 +785,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -789,7 +814,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -916,6 +941,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="43" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1261,32 +1291,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q48"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="41" zoomScaleNormal="41" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="99" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" customWidth="1"/>
-    <col min="8" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.81640625" customWidth="1"/>
-    <col min="14" max="14" width="74.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="74.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>1</v>
       </c>
@@ -1318,7 +1348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="57"/>
       <c r="B4" s="59"/>
       <c r="C4" s="61"/>
@@ -1356,7 +1386,7 @@
       <c r="O4" s="63"/>
       <c r="P4" s="55"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1.1000000000000001</v>
       </c>
@@ -1397,15 +1427,17 @@
         <v>5</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="12"/>
+        <v>51</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="P5" s="13" t="str">
         <f>IF(O5=N5,"PASS","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="16"/>
@@ -1440,15 +1472,17 @@
         <v>5</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="O6" s="12"/>
+        <v>52</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="P6" s="13" t="str">
         <f t="shared" ref="P6:P33" si="0">IF(O6=N6,"PASS","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
@@ -1483,15 +1517,17 @@
         <v>5</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="O7" s="12"/>
+        <v>53</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="P7" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19"/>
       <c r="B8" s="20"/>
       <c r="C8" s="21"/>
@@ -1525,65 +1561,67 @@
       <c r="M8" s="23">
         <v>5</v>
       </c>
-      <c r="N8" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="O8" s="24"/>
-      <c r="P8" s="13" t="str">
+      <c r="N8" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="O8" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="P8" s="67" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>1.2</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="25">
+        <v>100000</v>
+      </c>
+      <c r="E9" s="26">
+        <v>100000</v>
+      </c>
+      <c r="F9" s="26">
+        <v>0</v>
+      </c>
+      <c r="G9" s="26">
+        <v>0</v>
+      </c>
+      <c r="H9" s="26">
+        <v>10</v>
+      </c>
+      <c r="I9" s="26">
+        <v>15</v>
+      </c>
+      <c r="J9" s="26">
+        <v>0</v>
+      </c>
+      <c r="K9" s="26">
+        <v>1</v>
+      </c>
+      <c r="L9" s="26">
+        <v>5</v>
+      </c>
+      <c r="M9" s="26">
+        <v>5</v>
+      </c>
+      <c r="N9" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="27"/>
+      <c r="P9" s="38" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14">
-        <v>1.2</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="25">
-        <v>100000</v>
-      </c>
-      <c r="E9" s="26">
-        <v>100000</v>
-      </c>
-      <c r="F9" s="26">
-        <v>0</v>
-      </c>
-      <c r="G9" s="26">
-        <v>0</v>
-      </c>
-      <c r="H9" s="26">
-        <v>10</v>
-      </c>
-      <c r="I9" s="26">
-        <v>15</v>
-      </c>
-      <c r="J9" s="26">
-        <v>0</v>
-      </c>
-      <c r="K9" s="26">
-        <v>1</v>
-      </c>
-      <c r="L9" s="26">
-        <v>5</v>
-      </c>
-      <c r="M9" s="26">
-        <v>5</v>
-      </c>
-      <c r="N9" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9" s="27"/>
-      <c r="P9" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -1618,7 +1656,7 @@
         <v>5</v>
       </c>
       <c r="N10" s="30" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="O10" s="30"/>
       <c r="P10" s="13" t="str">
@@ -1626,7 +1664,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -1661,7 +1699,7 @@
         <v>5</v>
       </c>
       <c r="N11" s="30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O11" s="30"/>
       <c r="P11" s="13" t="str">
@@ -1669,7 +1707,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -1704,7 +1742,7 @@
         <v>5</v>
       </c>
       <c r="N12" s="30" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="O12" s="30"/>
       <c r="P12" s="13" t="str">
@@ -1712,7 +1750,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1738,24 +1776,26 @@
         <v>0</v>
       </c>
       <c r="K13" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" s="29">
         <v>0</v>
       </c>
       <c r="M13" s="29">
-        <v>5</v>
-      </c>
-      <c r="N13" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13" s="30"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="O13" s="30" t="s">
+        <v>55</v>
+      </c>
       <c r="P13" s="13" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -1790,15 +1830,17 @@
         <v>5</v>
       </c>
       <c r="N14" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" s="30"/>
+        <v>22</v>
+      </c>
+      <c r="O14" s="30" t="s">
+        <v>22</v>
+      </c>
       <c r="P14" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -1833,64 +1875,68 @@
         <v>5</v>
       </c>
       <c r="N15" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="O15" s="33"/>
-      <c r="P15" s="13" t="str">
+        <v>23</v>
+      </c>
+      <c r="O15" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15" s="50" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="25">
+        <v>20</v>
+      </c>
+      <c r="E16" s="26">
+        <v>20</v>
+      </c>
+      <c r="F16" s="26">
+        <v>0</v>
+      </c>
+      <c r="G16" s="26">
+        <v>0</v>
+      </c>
+      <c r="H16" s="26">
+        <v>20</v>
+      </c>
+      <c r="I16" s="26">
+        <v>20</v>
+      </c>
+      <c r="J16" s="26">
+        <v>0</v>
+      </c>
+      <c r="K16" s="26">
+        <v>1</v>
+      </c>
+      <c r="L16" s="26">
+        <v>10</v>
+      </c>
+      <c r="M16" s="26">
+        <v>10</v>
+      </c>
+      <c r="N16" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="O16" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="P16" s="38" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7">
-        <v>1.3</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="25">
-        <v>20</v>
-      </c>
-      <c r="E16" s="26">
-        <v>20</v>
-      </c>
-      <c r="F16" s="26">
-        <v>0</v>
-      </c>
-      <c r="G16" s="26">
-        <v>0</v>
-      </c>
-      <c r="H16" s="26">
-        <v>20</v>
-      </c>
-      <c r="I16" s="26">
-        <v>20</v>
-      </c>
-      <c r="J16" s="26">
-        <v>0</v>
-      </c>
-      <c r="K16" s="26">
-        <v>1</v>
-      </c>
-      <c r="L16" s="26">
-        <v>10</v>
-      </c>
-      <c r="M16" s="26">
-        <v>10</v>
-      </c>
-      <c r="N16" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="O16" s="27"/>
-      <c r="P16" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -1924,16 +1970,18 @@
       <c r="M17" s="29">
         <v>10</v>
       </c>
-      <c r="N17" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="O17" s="30"/>
+      <c r="N17" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="O17" s="27" t="s">
+        <v>55</v>
+      </c>
       <c r="P17" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -1967,16 +2015,18 @@
       <c r="M18" s="26">
         <v>10</v>
       </c>
-      <c r="N18" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="O18" s="30"/>
+      <c r="N18" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="O18" s="27" t="s">
+        <v>55</v>
+      </c>
       <c r="P18" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -2010,16 +2060,18 @@
       <c r="M19" s="29">
         <v>10</v>
       </c>
-      <c r="N19" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="O19" s="30"/>
+      <c r="N19" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="O19" s="27" t="s">
+        <v>55</v>
+      </c>
       <c r="P19" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -2054,15 +2106,17 @@
         <v>10</v>
       </c>
       <c r="N20" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="O20" s="30"/>
+        <v>58</v>
+      </c>
+      <c r="O20" s="30" t="s">
+        <v>58</v>
+      </c>
       <c r="P20" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -2096,16 +2150,18 @@
       <c r="M21" s="29">
         <v>10</v>
       </c>
-      <c r="N21" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="O21" s="30"/>
+      <c r="N21" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="O21" s="27" t="s">
+        <v>55</v>
+      </c>
       <c r="P21" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -2139,16 +2195,18 @@
       <c r="M22" s="26">
         <v>10</v>
       </c>
-      <c r="N22" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="O22" s="30"/>
+      <c r="N22" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="O22" s="27" t="s">
+        <v>55</v>
+      </c>
       <c r="P22" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -2182,19 +2240,21 @@
       <c r="M23" s="29">
         <v>10</v>
       </c>
-      <c r="N23" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="O23" s="30"/>
+      <c r="N23" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="O23" s="27" t="s">
+        <v>55</v>
+      </c>
       <c r="P23" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="16" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="28">
@@ -2228,15 +2288,17 @@
         <v>20</v>
       </c>
       <c r="N24" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="O24" s="30"/>
+        <v>58</v>
+      </c>
+      <c r="O24" s="30" t="s">
+        <v>57</v>
+      </c>
       <c r="P24" s="13" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -2271,15 +2333,17 @@
         <v>20</v>
       </c>
       <c r="N25" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O25" s="30"/>
+        <v>57</v>
+      </c>
+      <c r="O25" s="30" t="s">
+        <v>57</v>
+      </c>
       <c r="P25" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -2314,15 +2378,17 @@
         <v>21</v>
       </c>
       <c r="N26" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O26" s="30"/>
+        <v>57</v>
+      </c>
+      <c r="O26" s="30" t="s">
+        <v>57</v>
+      </c>
       <c r="P26" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -2357,15 +2423,17 @@
         <v>21</v>
       </c>
       <c r="N27" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O27" s="30"/>
+        <v>57</v>
+      </c>
+      <c r="O27" s="30" t="s">
+        <v>57</v>
+      </c>
       <c r="P27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -2399,16 +2467,18 @@
       <c r="M28" s="29">
         <v>0</v>
       </c>
-      <c r="N28" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="O28" s="30"/>
+      <c r="N28" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="O28" s="27" t="s">
+        <v>56</v>
+      </c>
       <c r="P28" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -2443,15 +2513,17 @@
         <v>0</v>
       </c>
       <c r="N29" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O29" s="30"/>
+        <v>57</v>
+      </c>
+      <c r="O29" s="30" t="s">
+        <v>57</v>
+      </c>
       <c r="P29" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -2486,15 +2558,17 @@
         <v>-1</v>
       </c>
       <c r="N30" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O30" s="30"/>
+        <v>57</v>
+      </c>
+      <c r="O30" s="30" t="s">
+        <v>57</v>
+      </c>
       <c r="P30" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -2528,24 +2602,26 @@
       <c r="M31" s="34">
         <v>-1</v>
       </c>
-      <c r="N31" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O31" s="30"/>
-      <c r="P31" s="13" t="str">
+      <c r="N31" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="O31" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="P31" s="67" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>1.4</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D32" s="18">
         <v>20</v>
@@ -2577,20 +2653,22 @@
       <c r="M32" s="26">
         <v>5</v>
       </c>
-      <c r="N32" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="O32" s="12"/>
-      <c r="P32" s="13" t="str">
+      <c r="N32" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="O32" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="P32" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D33" s="18">
         <v>20</v>
@@ -2623,20 +2701,22 @@
         <v>10</v>
       </c>
       <c r="N33" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="O33" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="O33" s="12" t="s">
+        <v>58</v>
+      </c>
       <c r="P33" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="56" t="s">
         <v>1</v>
       </c>
@@ -2668,7 +2748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="57"/>
       <c r="B38" s="59"/>
       <c r="C38" s="61"/>
@@ -2706,15 +2786,15 @@
       <c r="O38" s="63"/>
       <c r="P38" s="55"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
         <v>2.1</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D39" s="18">
         <v>20</v>
@@ -2747,15 +2827,17 @@
         <v>5</v>
       </c>
       <c r="N39" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="O39" s="11"/>
+        <v>45</v>
+      </c>
+      <c r="O39" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="P39" s="13" t="str">
         <f>IF(O39=N39,"PASS","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
@@ -2790,7 +2872,7 @@
         <v>5</v>
       </c>
       <c r="N40" s="41" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="O40" s="41"/>
       <c r="P40" s="13" t="str">
@@ -2798,7 +2880,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="42"/>
       <c r="B41" s="43"/>
       <c r="C41" s="44"/>
@@ -2833,24 +2915,26 @@
         <v>0</v>
       </c>
       <c r="N41" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="O41" s="45"/>
+        <v>59</v>
+      </c>
+      <c r="O41" s="45" t="s">
+        <v>59</v>
+      </c>
       <c r="P41" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="Q41" s="39"/>
     </row>
-    <row r="42" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48">
         <v>2.2000000000000002</v>
       </c>
       <c r="B42" s="47" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C42" s="49" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D42" s="18">
         <v>20</v>
@@ -2877,21 +2961,23 @@
         <v>1</v>
       </c>
       <c r="L42" s="18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M42" s="18">
         <v>5</v>
       </c>
       <c r="N42" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="O42" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="O42" s="12" t="s">
+        <v>46</v>
+      </c>
       <c r="P42" s="52" t="str">
         <f>IF(O42=N42,"PASS","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="C43" s="3"/>
@@ -2926,7 +3012,7 @@
         <v>100000</v>
       </c>
       <c r="N43" s="40" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="O43" s="40"/>
       <c r="P43" s="38" t="str">
@@ -2934,11 +3020,11 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="42"/>
       <c r="B44" s="43"/>
       <c r="C44" s="44" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D44" s="32">
         <v>20</v>
@@ -2971,23 +3057,25 @@
         <v>5</v>
       </c>
       <c r="N44" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="O44" s="45"/>
+        <v>50</v>
+      </c>
+      <c r="O44" s="45" t="s">
+        <v>50</v>
+      </c>
       <c r="P44" s="50" t="str">
         <f t="shared" si="2"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
         <v>2.2999999999999998</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D45" s="23">
         <v>20</v>
@@ -3020,64 +3108,68 @@
         <v>5</v>
       </c>
       <c r="N45" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="O45" s="24"/>
+        <v>47</v>
+      </c>
+      <c r="O45" s="24" t="s">
+        <v>47</v>
+      </c>
       <c r="P45" s="51" t="str">
         <f t="shared" ref="P45:P48" si="3">IF(O45=N45,"PASS","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14">
         <v>2.4</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C46" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" s="18">
+        <v>20</v>
+      </c>
+      <c r="E46" s="18">
+        <v>20</v>
+      </c>
+      <c r="F46" s="18">
+        <v>0</v>
+      </c>
+      <c r="G46" s="18">
+        <v>0</v>
+      </c>
+      <c r="H46" s="18">
+        <v>0</v>
+      </c>
+      <c r="I46" s="18">
+        <v>0</v>
+      </c>
+      <c r="J46" s="18">
+        <v>0</v>
+      </c>
+      <c r="K46" s="18">
+        <v>1</v>
+      </c>
+      <c r="L46" s="18">
+        <v>5</v>
+      </c>
+      <c r="M46" s="18">
+        <v>5</v>
+      </c>
+      <c r="N46" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D46" s="18">
-        <v>20</v>
-      </c>
-      <c r="E46" s="18">
-        <v>20</v>
-      </c>
-      <c r="F46" s="18">
-        <v>0</v>
-      </c>
-      <c r="G46" s="18">
-        <v>0</v>
-      </c>
-      <c r="H46" s="18">
-        <v>0</v>
-      </c>
-      <c r="I46" s="18">
-        <v>0</v>
-      </c>
-      <c r="J46" s="18">
-        <v>0</v>
-      </c>
-      <c r="K46" s="18">
-        <v>1</v>
-      </c>
-      <c r="L46" s="18">
-        <v>5</v>
-      </c>
-      <c r="M46" s="18">
-        <v>5</v>
-      </c>
-      <c r="N46" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O46" s="12"/>
+      <c r="O46" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="P46" s="38" t="str">
         <f t="shared" si="3"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="19"/>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
@@ -3111,24 +3203,26 @@
       <c r="M47" s="23">
         <v>0</v>
       </c>
-      <c r="N47" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="O47" s="24"/>
+      <c r="N47" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="O47" s="24" t="s">
+        <v>49</v>
+      </c>
       <c r="P47" s="53" t="str">
         <f t="shared" si="3"/>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14">
         <v>2.5</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D48" s="26">
         <v>20</v>
@@ -3161,16 +3255,25 @@
         <v>5</v>
       </c>
       <c r="N48" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="O48" s="27"/>
+        <v>41</v>
+      </c>
+      <c r="O48" s="27" t="s">
+        <v>41</v>
+      </c>
       <c r="P48" s="38" t="str">
         <f t="shared" si="3"/>
-        <v>FAIL</v>
-      </c>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="69"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="C51:C52"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="B37:B38"/>

</xml_diff>